<commit_message>
Fix UploadTemplate and data_dictionary download files
</commit_message>
<xml_diff>
--- a/public/UploadResources/HLA_COVID19_data_dictionary.xlsx
+++ b/public/UploadResources/HLA_COVID19_data_dictionary.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arenschen/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arenschen/ucsf_dev_repos/hlacovid_rails/hlacovid19/public/UploadResources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{685650EA-BECA-9543-8E37-A93DEACAE4F4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55FD8CAE-3C9F-754A-95EC-F4B0944104FF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2040" yWindow="460" windowWidth="20220" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{EE76B065-1B3F-D242-A982-718FAF7E31AC}" name="comorbs5" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/arenschen/Desktop/comorbs5.txt" space="1" consecutive="1">
+    <textPr sourceFile="/Users/arenschen/Desktop/comorbs5.txt" space="1" consecutive="1">
       <textFields count="2">
         <textField/>
         <textField/>
@@ -846,6 +846,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -867,18 +879,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1102,7 +1102,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
       <selection activeCell="G174" sqref="G174"/>
     </sheetView>
   </sheetViews>
@@ -1131,7 +1131,7 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="22" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -1148,7 +1148,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="13"/>
+      <c r="A3" s="19"/>
       <c r="B3" s="5" t="s">
         <v>9</v>
       </c>
@@ -1160,7 +1160,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="13"/>
+      <c r="A4" s="19"/>
       <c r="B4" s="5" t="s">
         <v>10</v>
       </c>
@@ -1172,7 +1172,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="13"/>
+      <c r="A5" s="19"/>
       <c r="B5" s="5" t="s">
         <v>11</v>
       </c>
@@ -1184,7 +1184,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="13"/>
+      <c r="A6" s="19"/>
       <c r="B6" s="5" t="s">
         <v>13</v>
       </c>
@@ -1196,7 +1196,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="13"/>
+      <c r="A7" s="19"/>
       <c r="B7" s="5" t="s">
         <v>14</v>
       </c>
@@ -1208,7 +1208,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="13"/>
+      <c r="A8" s="19"/>
       <c r="B8" s="6" t="s">
         <v>16</v>
       </c>
@@ -1223,7 +1223,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="13"/>
+      <c r="A9" s="19"/>
       <c r="B9" s="6" t="s">
         <v>18</v>
       </c>
@@ -1238,7 +1238,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="13"/>
+      <c r="A10" s="19"/>
       <c r="B10" s="6" t="s">
         <v>20</v>
       </c>
@@ -1253,7 +1253,7 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="13"/>
+      <c r="A11" s="19"/>
       <c r="B11" s="6" t="s">
         <v>21</v>
       </c>
@@ -1265,7 +1265,7 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="13"/>
+      <c r="A12" s="19"/>
       <c r="B12" s="6" t="s">
         <v>22</v>
       </c>
@@ -1277,7 +1277,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="14"/>
+      <c r="A13" s="20"/>
       <c r="B13" s="7" t="s">
         <v>23</v>
       </c>
@@ -1296,7 +1296,7 @@
       <c r="K13" s="7"/>
     </row>
     <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="17" t="s">
+      <c r="A14" s="23" t="s">
         <v>24</v>
       </c>
       <c r="B14" s="6" t="s">
@@ -1317,7 +1317,7 @@
       <c r="K14" s="6"/>
     </row>
     <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="13"/>
+      <c r="A15" s="19"/>
       <c r="B15" s="5" t="s">
         <v>26</v>
       </c>
@@ -1329,7 +1329,7 @@
       </c>
     </row>
     <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="13"/>
+      <c r="A16" s="19"/>
       <c r="B16" s="5" t="s">
         <v>27</v>
       </c>
@@ -1341,7 +1341,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="13"/>
+      <c r="A17" s="19"/>
       <c r="B17" s="5" t="s">
         <v>28</v>
       </c>
@@ -1353,7 +1353,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="13"/>
+      <c r="A18" s="19"/>
       <c r="B18" s="5" t="s">
         <v>29</v>
       </c>
@@ -1365,7 +1365,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="13"/>
+      <c r="A19" s="19"/>
       <c r="B19" s="5" t="s">
         <v>30</v>
       </c>
@@ -1377,7 +1377,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="13"/>
+      <c r="A20" s="19"/>
       <c r="B20" s="5" t="s">
         <v>31</v>
       </c>
@@ -1389,7 +1389,7 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="13"/>
+      <c r="A21" s="19"/>
       <c r="B21" s="5" t="s">
         <v>32</v>
       </c>
@@ -1401,7 +1401,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="13"/>
+      <c r="A22" s="19"/>
       <c r="B22" s="5" t="s">
         <v>33</v>
       </c>
@@ -1413,7 +1413,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="13"/>
+      <c r="A23" s="19"/>
       <c r="B23" s="5" t="s">
         <v>34</v>
       </c>
@@ -1425,7 +1425,7 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="13"/>
+      <c r="A24" s="19"/>
       <c r="B24" s="5" t="s">
         <v>35</v>
       </c>
@@ -1437,7 +1437,7 @@
       </c>
     </row>
     <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="13"/>
+      <c r="A25" s="19"/>
       <c r="B25" s="5" t="s">
         <v>36</v>
       </c>
@@ -1449,7 +1449,7 @@
       </c>
     </row>
     <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="13"/>
+      <c r="A26" s="19"/>
       <c r="B26" s="5" t="s">
         <v>37</v>
       </c>
@@ -1461,7 +1461,7 @@
       </c>
     </row>
     <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="13"/>
+      <c r="A27" s="19"/>
       <c r="B27" s="5" t="s">
         <v>38</v>
       </c>
@@ -1473,7 +1473,7 @@
       </c>
     </row>
     <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="13"/>
+      <c r="A28" s="19"/>
       <c r="B28" s="5" t="s">
         <v>39</v>
       </c>
@@ -1485,7 +1485,7 @@
       </c>
     </row>
     <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="13"/>
+      <c r="A29" s="19"/>
       <c r="B29" s="5" t="s">
         <v>40</v>
       </c>
@@ -1497,7 +1497,7 @@
       </c>
     </row>
     <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="13"/>
+      <c r="A30" s="19"/>
       <c r="B30" s="5" t="s">
         <v>41</v>
       </c>
@@ -1512,7 +1512,7 @@
       </c>
     </row>
     <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="13"/>
+      <c r="A31" s="19"/>
       <c r="B31" s="5" t="s">
         <v>44</v>
       </c>
@@ -1527,7 +1527,7 @@
       </c>
     </row>
     <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="13"/>
+      <c r="A32" s="19"/>
       <c r="B32" s="5" t="s">
         <v>46</v>
       </c>
@@ -1542,7 +1542,7 @@
       </c>
     </row>
     <row r="33" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="13"/>
+      <c r="A33" s="19"/>
       <c r="B33" s="5" t="s">
         <v>48</v>
       </c>
@@ -1557,7 +1557,7 @@
       </c>
     </row>
     <row r="34" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="13"/>
+      <c r="A34" s="19"/>
       <c r="B34" s="5" t="s">
         <v>50</v>
       </c>
@@ -1572,7 +1572,7 @@
       </c>
     </row>
     <row r="35" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="13"/>
+      <c r="A35" s="19"/>
       <c r="B35" s="5" t="s">
         <v>53</v>
       </c>
@@ -1587,7 +1587,7 @@
       </c>
     </row>
     <row r="36" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="13"/>
+      <c r="A36" s="19"/>
       <c r="B36" s="5" t="s">
         <v>55</v>
       </c>
@@ -1602,7 +1602,7 @@
       </c>
     </row>
     <row r="37" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="13"/>
+      <c r="A37" s="19"/>
       <c r="B37" s="5" t="s">
         <v>57</v>
       </c>
@@ -1617,7 +1617,7 @@
       </c>
     </row>
     <row r="38" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="13"/>
+      <c r="A38" s="19"/>
       <c r="B38" s="5" t="s">
         <v>59</v>
       </c>
@@ -1632,7 +1632,7 @@
       </c>
     </row>
     <row r="39" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="14"/>
+      <c r="A39" s="20"/>
       <c r="B39" s="9" t="s">
         <v>61</v>
       </c>
@@ -1668,7 +1668,7 @@
       <c r="Z39" s="9"/>
     </row>
     <row r="40" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="18" t="s">
+      <c r="A40" s="24" t="s">
         <v>63</v>
       </c>
       <c r="B40" s="6" t="s">
@@ -1682,7 +1682,7 @@
       </c>
     </row>
     <row r="41" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="13"/>
+      <c r="A41" s="19"/>
       <c r="B41" s="6" t="s">
         <v>66</v>
       </c>
@@ -1694,7 +1694,7 @@
       </c>
     </row>
     <row r="42" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="13"/>
+      <c r="A42" s="19"/>
       <c r="B42" s="5" t="s">
         <v>67</v>
       </c>
@@ -1706,7 +1706,7 @@
       </c>
     </row>
     <row r="43" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="13"/>
+      <c r="A43" s="19"/>
       <c r="B43" s="5" t="s">
         <v>68</v>
       </c>
@@ -1718,7 +1718,7 @@
       </c>
     </row>
     <row r="44" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="13"/>
+      <c r="A44" s="19"/>
       <c r="B44" s="5" t="s">
         <v>69</v>
       </c>
@@ -1730,7 +1730,7 @@
       </c>
     </row>
     <row r="45" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="13"/>
+      <c r="A45" s="19"/>
       <c r="B45" s="5" t="s">
         <v>70</v>
       </c>
@@ -1742,7 +1742,7 @@
       </c>
     </row>
     <row r="46" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="13"/>
+      <c r="A46" s="19"/>
       <c r="B46" s="5" t="s">
         <v>71</v>
       </c>
@@ -1754,7 +1754,7 @@
       </c>
     </row>
     <row r="47" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="13"/>
+      <c r="A47" s="19"/>
       <c r="B47" s="5" t="s">
         <v>72</v>
       </c>
@@ -1766,7 +1766,7 @@
       </c>
     </row>
     <row r="48" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="13"/>
+      <c r="A48" s="19"/>
       <c r="B48" s="5" t="s">
         <v>73</v>
       </c>
@@ -1778,7 +1778,7 @@
       </c>
     </row>
     <row r="49" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="13"/>
+      <c r="A49" s="19"/>
       <c r="B49" s="5" t="s">
         <v>74</v>
       </c>
@@ -1790,7 +1790,7 @@
       </c>
     </row>
     <row r="50" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="13"/>
+      <c r="A50" s="19"/>
       <c r="B50" s="5" t="s">
         <v>75</v>
       </c>
@@ -1802,7 +1802,7 @@
       </c>
     </row>
     <row r="51" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="13"/>
+      <c r="A51" s="19"/>
       <c r="B51" s="5" t="s">
         <v>76</v>
       </c>
@@ -1814,7 +1814,7 @@
       </c>
     </row>
     <row r="52" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="13"/>
+      <c r="A52" s="19"/>
       <c r="B52" s="5" t="s">
         <v>77</v>
       </c>
@@ -1826,7 +1826,7 @@
       </c>
     </row>
     <row r="53" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="13"/>
+      <c r="A53" s="19"/>
       <c r="B53" s="5" t="s">
         <v>78</v>
       </c>
@@ -1838,7 +1838,7 @@
       </c>
     </row>
     <row r="54" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="13"/>
+      <c r="A54" s="19"/>
       <c r="B54" s="5" t="s">
         <v>79</v>
       </c>
@@ -1850,7 +1850,7 @@
       </c>
     </row>
     <row r="55" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="13"/>
+      <c r="A55" s="19"/>
       <c r="B55" s="5" t="s">
         <v>80</v>
       </c>
@@ -1862,7 +1862,7 @@
       </c>
     </row>
     <row r="56" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="13"/>
+      <c r="A56" s="19"/>
       <c r="B56" s="5" t="s">
         <v>81</v>
       </c>
@@ -1874,7 +1874,7 @@
       </c>
     </row>
     <row r="57" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="14"/>
+      <c r="A57" s="20"/>
       <c r="B57" s="9" t="s">
         <v>82</v>
       </c>
@@ -1908,7 +1908,7 @@
       <c r="Z57" s="9"/>
     </row>
     <row r="58" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="19" t="s">
+      <c r="A58" s="25" t="s">
         <v>83</v>
       </c>
       <c r="B58" s="5" t="s">
@@ -1922,7 +1922,7 @@
       </c>
     </row>
     <row r="59" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="13"/>
+      <c r="A59" s="19"/>
       <c r="B59" s="5" t="s">
         <v>85</v>
       </c>
@@ -1934,7 +1934,7 @@
       </c>
     </row>
     <row r="60" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="13"/>
+      <c r="A60" s="19"/>
       <c r="B60" s="6" t="s">
         <v>86</v>
       </c>
@@ -1946,7 +1946,7 @@
       </c>
     </row>
     <row r="61" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="13"/>
+      <c r="A61" s="19"/>
       <c r="B61" s="5" t="s">
         <v>87</v>
       </c>
@@ -1958,7 +1958,7 @@
       </c>
     </row>
     <row r="62" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="13"/>
+      <c r="A62" s="19"/>
       <c r="B62" s="5" t="s">
         <v>88</v>
       </c>
@@ -1970,7 +1970,7 @@
       </c>
     </row>
     <row r="63" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="13"/>
+      <c r="A63" s="19"/>
       <c r="B63" s="5" t="s">
         <v>89</v>
       </c>
@@ -1982,7 +1982,7 @@
       </c>
     </row>
     <row r="64" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="13"/>
+      <c r="A64" s="19"/>
       <c r="B64" s="5" t="s">
         <v>90</v>
       </c>
@@ -1994,7 +1994,7 @@
       </c>
     </row>
     <row r="65" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="13"/>
+      <c r="A65" s="19"/>
       <c r="B65" s="5" t="s">
         <v>91</v>
       </c>
@@ -2006,7 +2006,7 @@
       </c>
     </row>
     <row r="66" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="13"/>
+      <c r="A66" s="19"/>
       <c r="B66" s="5" t="s">
         <v>92</v>
       </c>
@@ -2018,7 +2018,7 @@
       </c>
     </row>
     <row r="67" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="13"/>
+      <c r="A67" s="19"/>
       <c r="B67" s="5" t="s">
         <v>93</v>
       </c>
@@ -2030,7 +2030,7 @@
       </c>
     </row>
     <row r="68" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="13"/>
+      <c r="A68" s="19"/>
       <c r="B68" s="5" t="s">
         <v>94</v>
       </c>
@@ -2042,7 +2042,7 @@
       </c>
     </row>
     <row r="69" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="13"/>
+      <c r="A69" s="19"/>
       <c r="B69" s="5" t="s">
         <v>95</v>
       </c>
@@ -2054,7 +2054,7 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="13"/>
+      <c r="A70" s="19"/>
       <c r="B70" s="5" t="s">
         <v>96</v>
       </c>
@@ -2066,7 +2066,7 @@
       </c>
     </row>
     <row r="71" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="13"/>
+      <c r="A71" s="19"/>
       <c r="B71" s="5" t="s">
         <v>97</v>
       </c>
@@ -2078,7 +2078,7 @@
       </c>
     </row>
     <row r="72" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="13"/>
+      <c r="A72" s="19"/>
       <c r="B72" s="5" t="s">
         <v>98</v>
       </c>
@@ -2090,7 +2090,7 @@
       </c>
     </row>
     <row r="73" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="13"/>
+      <c r="A73" s="19"/>
       <c r="B73" s="5" t="s">
         <v>99</v>
       </c>
@@ -2102,7 +2102,7 @@
       </c>
     </row>
     <row r="74" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="13"/>
+      <c r="A74" s="19"/>
       <c r="B74" s="5" t="s">
         <v>100</v>
       </c>
@@ -2114,7 +2114,7 @@
       </c>
     </row>
     <row r="75" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="13"/>
+      <c r="A75" s="19"/>
       <c r="B75" s="5" t="s">
         <v>101</v>
       </c>
@@ -2126,7 +2126,7 @@
       </c>
     </row>
     <row r="76" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="13"/>
+      <c r="A76" s="19"/>
       <c r="B76" s="5" t="s">
         <v>102</v>
       </c>
@@ -2138,7 +2138,7 @@
       </c>
     </row>
     <row r="77" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="13"/>
+      <c r="A77" s="19"/>
       <c r="B77" s="5" t="s">
         <v>103</v>
       </c>
@@ -2150,7 +2150,7 @@
       </c>
     </row>
     <row r="78" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="13"/>
+      <c r="A78" s="19"/>
       <c r="B78" s="5" t="s">
         <v>104</v>
       </c>
@@ -2162,7 +2162,7 @@
       </c>
     </row>
     <row r="79" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="13"/>
+      <c r="A79" s="19"/>
       <c r="B79" s="5" t="s">
         <v>105</v>
       </c>
@@ -2174,7 +2174,7 @@
       </c>
     </row>
     <row r="80" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="13"/>
+      <c r="A80" s="19"/>
       <c r="B80" s="5" t="s">
         <v>106</v>
       </c>
@@ -2186,7 +2186,7 @@
       </c>
     </row>
     <row r="81" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="13"/>
+      <c r="A81" s="19"/>
       <c r="B81" s="5" t="s">
         <v>107</v>
       </c>
@@ -2198,7 +2198,7 @@
       </c>
     </row>
     <row r="82" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="13"/>
+      <c r="A82" s="19"/>
       <c r="B82" s="5" t="s">
         <v>108</v>
       </c>
@@ -2210,7 +2210,7 @@
       </c>
     </row>
     <row r="83" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="13"/>
+      <c r="A83" s="19"/>
       <c r="B83" s="5" t="s">
         <v>109</v>
       </c>
@@ -2222,7 +2222,7 @@
       </c>
     </row>
     <row r="84" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="14"/>
+      <c r="A84" s="20"/>
       <c r="B84" s="9" t="s">
         <v>110</v>
       </c>
@@ -2256,7 +2256,7 @@
       <c r="Z84" s="9"/>
     </row>
     <row r="85" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="20" t="s">
+      <c r="A85" s="26" t="s">
         <v>111</v>
       </c>
       <c r="B85" s="6" t="s">
@@ -2270,7 +2270,7 @@
       </c>
     </row>
     <row r="86" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="13"/>
+      <c r="A86" s="19"/>
       <c r="B86" s="5" t="s">
         <v>113</v>
       </c>
@@ -2282,7 +2282,7 @@
       </c>
     </row>
     <row r="87" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="13"/>
+      <c r="A87" s="19"/>
       <c r="B87" s="5" t="s">
         <v>114</v>
       </c>
@@ -2294,7 +2294,7 @@
       </c>
     </row>
     <row r="88" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="14"/>
+      <c r="A88" s="20"/>
       <c r="B88" s="9" t="s">
         <v>115</v>
       </c>
@@ -2328,7 +2328,7 @@
       <c r="Z88" s="9"/>
     </row>
     <row r="89" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="12" t="s">
+      <c r="A89" s="18" t="s">
         <v>116</v>
       </c>
       <c r="B89" s="5" t="s">
@@ -2342,7 +2342,7 @@
       </c>
     </row>
     <row r="90" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="13"/>
+      <c r="A90" s="19"/>
       <c r="B90" s="5" t="s">
         <v>118</v>
       </c>
@@ -2354,7 +2354,7 @@
       </c>
     </row>
     <row r="91" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="13"/>
+      <c r="A91" s="19"/>
       <c r="B91" s="5" t="s">
         <v>119</v>
       </c>
@@ -2366,7 +2366,7 @@
       </c>
     </row>
     <row r="92" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="13"/>
+      <c r="A92" s="19"/>
       <c r="B92" s="5" t="s">
         <v>120</v>
       </c>
@@ -2378,7 +2378,7 @@
       </c>
     </row>
     <row r="93" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="13"/>
+      <c r="A93" s="19"/>
       <c r="B93" s="5" t="s">
         <v>121</v>
       </c>
@@ -2390,7 +2390,7 @@
       </c>
     </row>
     <row r="94" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="13"/>
+      <c r="A94" s="19"/>
       <c r="B94" s="5" t="s">
         <v>122</v>
       </c>
@@ -2402,7 +2402,7 @@
       </c>
     </row>
     <row r="95" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="13"/>
+      <c r="A95" s="19"/>
       <c r="B95" s="5" t="s">
         <v>123</v>
       </c>
@@ -2414,7 +2414,7 @@
       </c>
     </row>
     <row r="96" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="13"/>
+      <c r="A96" s="19"/>
       <c r="B96" s="5" t="s">
         <v>124</v>
       </c>
@@ -2426,7 +2426,7 @@
       </c>
     </row>
     <row r="97" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="13"/>
+      <c r="A97" s="19"/>
       <c r="B97" s="5" t="s">
         <v>125</v>
       </c>
@@ -2438,7 +2438,7 @@
       </c>
     </row>
     <row r="98" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="13"/>
+      <c r="A98" s="19"/>
       <c r="B98" s="5" t="s">
         <v>126</v>
       </c>
@@ -2450,7 +2450,7 @@
       </c>
     </row>
     <row r="99" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="13"/>
+      <c r="A99" s="19"/>
       <c r="B99" s="5" t="s">
         <v>127</v>
       </c>
@@ -2462,7 +2462,7 @@
       </c>
     </row>
     <row r="100" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="13"/>
+      <c r="A100" s="19"/>
       <c r="B100" s="5" t="s">
         <v>128</v>
       </c>
@@ -2474,7 +2474,7 @@
       </c>
     </row>
     <row r="101" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="13"/>
+      <c r="A101" s="19"/>
       <c r="B101" s="5" t="s">
         <v>129</v>
       </c>
@@ -2486,7 +2486,7 @@
       </c>
     </row>
     <row r="102" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="13"/>
+      <c r="A102" s="19"/>
       <c r="B102" s="5" t="s">
         <v>130</v>
       </c>
@@ -2498,7 +2498,7 @@
       </c>
     </row>
     <row r="103" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A103" s="13"/>
+      <c r="A103" s="19"/>
       <c r="B103" s="5" t="s">
         <v>131</v>
       </c>
@@ -2510,7 +2510,7 @@
       </c>
     </row>
     <row r="104" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="13"/>
+      <c r="A104" s="19"/>
       <c r="B104" s="5" t="s">
         <v>132</v>
       </c>
@@ -2522,7 +2522,7 @@
       </c>
     </row>
     <row r="105" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A105" s="13"/>
+      <c r="A105" s="19"/>
       <c r="B105" s="5" t="s">
         <v>133</v>
       </c>
@@ -2534,7 +2534,7 @@
       </c>
     </row>
     <row r="106" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="13"/>
+      <c r="A106" s="19"/>
       <c r="B106" s="5" t="s">
         <v>134</v>
       </c>
@@ -2546,7 +2546,7 @@
       </c>
     </row>
     <row r="107" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="13"/>
+      <c r="A107" s="19"/>
       <c r="B107" s="5" t="s">
         <v>135</v>
       </c>
@@ -2558,7 +2558,7 @@
       </c>
     </row>
     <row r="108" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="13"/>
+      <c r="A108" s="19"/>
       <c r="B108" s="5" t="s">
         <v>136</v>
       </c>
@@ -2570,7 +2570,7 @@
       </c>
     </row>
     <row r="109" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A109" s="13"/>
+      <c r="A109" s="19"/>
       <c r="B109" s="5" t="s">
         <v>137</v>
       </c>
@@ -2582,7 +2582,7 @@
       </c>
     </row>
     <row r="110" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="13"/>
+      <c r="A110" s="19"/>
       <c r="B110" s="5" t="s">
         <v>138</v>
       </c>
@@ -2594,7 +2594,7 @@
       </c>
     </row>
     <row r="111" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A111" s="13"/>
+      <c r="A111" s="19"/>
       <c r="B111" s="5" t="s">
         <v>139</v>
       </c>
@@ -2606,7 +2606,7 @@
       </c>
     </row>
     <row r="112" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A112" s="13"/>
+      <c r="A112" s="19"/>
       <c r="B112" s="5" t="s">
         <v>140</v>
       </c>
@@ -2618,7 +2618,7 @@
       </c>
     </row>
     <row r="113" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A113" s="13"/>
+      <c r="A113" s="19"/>
       <c r="B113" s="5" t="s">
         <v>141</v>
       </c>
@@ -2630,7 +2630,7 @@
       </c>
     </row>
     <row r="114" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A114" s="13"/>
+      <c r="A114" s="19"/>
       <c r="B114" s="5" t="s">
         <v>142</v>
       </c>
@@ -2642,7 +2642,7 @@
       </c>
     </row>
     <row r="115" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A115" s="13"/>
+      <c r="A115" s="19"/>
       <c r="B115" s="5" t="s">
         <v>143</v>
       </c>
@@ -2654,7 +2654,7 @@
       </c>
     </row>
     <row r="116" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A116" s="13"/>
+      <c r="A116" s="19"/>
       <c r="B116" s="5" t="s">
         <v>144</v>
       </c>
@@ -2666,7 +2666,7 @@
       </c>
     </row>
     <row r="117" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A117" s="13"/>
+      <c r="A117" s="19"/>
       <c r="B117" s="5" t="s">
         <v>145</v>
       </c>
@@ -2678,7 +2678,7 @@
       </c>
     </row>
     <row r="118" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A118" s="13"/>
+      <c r="A118" s="19"/>
       <c r="B118" s="5" t="s">
         <v>146</v>
       </c>
@@ -2690,7 +2690,7 @@
       </c>
     </row>
     <row r="119" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A119" s="13"/>
+      <c r="A119" s="19"/>
       <c r="B119" s="5" t="s">
         <v>147</v>
       </c>
@@ -2702,7 +2702,7 @@
       </c>
     </row>
     <row r="120" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A120" s="13"/>
+      <c r="A120" s="19"/>
       <c r="B120" s="5" t="s">
         <v>148</v>
       </c>
@@ -2714,7 +2714,7 @@
       </c>
     </row>
     <row r="121" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A121" s="13"/>
+      <c r="A121" s="19"/>
       <c r="B121" s="5" t="s">
         <v>149</v>
       </c>
@@ -2726,7 +2726,7 @@
       </c>
     </row>
     <row r="122" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A122" s="14"/>
+      <c r="A122" s="20"/>
       <c r="B122" s="9" t="s">
         <v>150</v>
       </c>
@@ -2760,7 +2760,7 @@
       <c r="Z122" s="9"/>
     </row>
     <row r="123" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A123" s="15" t="s">
+      <c r="A123" s="21" t="s">
         <v>151</v>
       </c>
       <c r="B123" s="5" t="s">
@@ -2774,7 +2774,7 @@
       </c>
     </row>
     <row r="124" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A124" s="13"/>
+      <c r="A124" s="19"/>
       <c r="B124" s="5" t="s">
         <v>153</v>
       </c>
@@ -2786,7 +2786,7 @@
       </c>
     </row>
     <row r="125" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A125" s="13"/>
+      <c r="A125" s="19"/>
       <c r="B125" s="5" t="s">
         <v>154</v>
       </c>
@@ -2798,7 +2798,7 @@
       </c>
     </row>
     <row r="126" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A126" s="13"/>
+      <c r="A126" s="19"/>
       <c r="B126" s="5" t="s">
         <v>155</v>
       </c>
@@ -2810,7 +2810,7 @@
       </c>
     </row>
     <row r="127" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A127" s="13"/>
+      <c r="A127" s="19"/>
       <c r="B127" s="5" t="s">
         <v>156</v>
       </c>
@@ -2822,7 +2822,7 @@
       </c>
     </row>
     <row r="128" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A128" s="13"/>
+      <c r="A128" s="19"/>
       <c r="B128" s="5" t="s">
         <v>157</v>
       </c>
@@ -2834,7 +2834,7 @@
       </c>
     </row>
     <row r="129" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A129" s="13"/>
+      <c r="A129" s="19"/>
       <c r="B129" s="5" t="s">
         <v>158</v>
       </c>
@@ -2846,7 +2846,7 @@
       </c>
     </row>
     <row r="130" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A130" s="13"/>
+      <c r="A130" s="19"/>
       <c r="B130" s="5" t="s">
         <v>159</v>
       </c>
@@ -2858,7 +2858,7 @@
       </c>
     </row>
     <row r="131" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A131" s="13"/>
+      <c r="A131" s="19"/>
       <c r="B131" s="5" t="s">
         <v>160</v>
       </c>
@@ -2870,7 +2870,7 @@
       </c>
     </row>
     <row r="132" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A132" s="13"/>
+      <c r="A132" s="19"/>
       <c r="B132" s="5" t="s">
         <v>161</v>
       </c>
@@ -2882,7 +2882,7 @@
       </c>
     </row>
     <row r="133" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A133" s="13"/>
+      <c r="A133" s="19"/>
       <c r="B133" s="5" t="s">
         <v>162</v>
       </c>
@@ -2894,7 +2894,7 @@
       </c>
     </row>
     <row r="134" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A134" s="13"/>
+      <c r="A134" s="19"/>
       <c r="B134" s="5" t="s">
         <v>163</v>
       </c>
@@ -2906,7 +2906,7 @@
       </c>
     </row>
     <row r="135" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A135" s="13"/>
+      <c r="A135" s="19"/>
       <c r="B135" s="5" t="s">
         <v>164</v>
       </c>
@@ -2918,7 +2918,7 @@
       </c>
     </row>
     <row r="136" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A136" s="13"/>
+      <c r="A136" s="19"/>
       <c r="B136" s="5" t="s">
         <v>165</v>
       </c>
@@ -2930,7 +2930,7 @@
       </c>
     </row>
     <row r="137" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A137" s="13"/>
+      <c r="A137" s="19"/>
       <c r="B137" s="5" t="s">
         <v>166</v>
       </c>
@@ -2942,7 +2942,7 @@
       </c>
     </row>
     <row r="138" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A138" s="13"/>
+      <c r="A138" s="19"/>
       <c r="B138" s="5" t="s">
         <v>167</v>
       </c>
@@ -2954,7 +2954,7 @@
       </c>
     </row>
     <row r="139" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A139" s="14"/>
+      <c r="A139" s="20"/>
       <c r="B139" s="9" t="s">
         <v>168</v>
       </c>
@@ -2988,274 +2988,274 @@
       <c r="Z139" s="9"/>
     </row>
     <row r="140" spans="1:26" ht="16" x14ac:dyDescent="0.2">
-      <c r="A140" s="22" t="s">
+      <c r="A140" s="15" t="s">
         <v>200</v>
       </c>
-      <c r="B140" s="21" t="s">
+      <c r="B140" s="12" t="s">
         <v>169</v>
       </c>
-      <c r="C140" s="21" t="s">
+      <c r="C140" s="12" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="141" spans="1:26" ht="16" x14ac:dyDescent="0.2">
-      <c r="A141" s="23"/>
-      <c r="B141" s="21" t="s">
+      <c r="A141" s="16"/>
+      <c r="B141" s="12" t="s">
         <v>170</v>
       </c>
-      <c r="C141" s="21" t="s">
+      <c r="C141" s="12" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="142" spans="1:26" ht="16" x14ac:dyDescent="0.2">
-      <c r="A142" s="23"/>
-      <c r="B142" s="21" t="s">
+      <c r="A142" s="16"/>
+      <c r="B142" s="12" t="s">
         <v>172</v>
       </c>
-      <c r="C142" s="21" t="s">
+      <c r="C142" s="12" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="143" spans="1:26" ht="16" x14ac:dyDescent="0.2">
-      <c r="A143" s="23"/>
-      <c r="B143" s="21" t="s">
+      <c r="A143" s="16"/>
+      <c r="B143" s="12" t="s">
         <v>173</v>
       </c>
-      <c r="C143" s="21" t="s">
+      <c r="C143" s="12" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="144" spans="1:26" ht="16" x14ac:dyDescent="0.2">
-      <c r="A144" s="23"/>
-      <c r="B144" s="21" t="s">
+      <c r="A144" s="16"/>
+      <c r="B144" s="12" t="s">
         <v>174</v>
       </c>
-      <c r="C144" s="21" t="s">
+      <c r="C144" s="12" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="145" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A145" s="23"/>
-      <c r="B145" s="21" t="s">
+      <c r="A145" s="16"/>
+      <c r="B145" s="12" t="s">
         <v>175</v>
       </c>
-      <c r="C145" s="21" t="s">
+      <c r="C145" s="12" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="146" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A146" s="23"/>
-      <c r="B146" s="21" t="s">
+      <c r="A146" s="16"/>
+      <c r="B146" s="12" t="s">
         <v>176</v>
       </c>
-      <c r="C146" s="21" t="s">
+      <c r="C146" s="12" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="147" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A147" s="23"/>
-      <c r="B147" s="21" t="s">
+      <c r="A147" s="16"/>
+      <c r="B147" s="12" t="s">
         <v>177</v>
       </c>
-      <c r="C147" s="21" t="s">
+      <c r="C147" s="12" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="148" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A148" s="23"/>
-      <c r="B148" s="21" t="s">
+      <c r="A148" s="16"/>
+      <c r="B148" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="C148" s="21" t="s">
+      <c r="C148" s="12" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="149" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A149" s="23"/>
-      <c r="B149" s="21" t="s">
+      <c r="A149" s="16"/>
+      <c r="B149" s="12" t="s">
         <v>179</v>
       </c>
-      <c r="C149" s="21" t="s">
+      <c r="C149" s="12" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="150" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A150" s="23"/>
-      <c r="B150" s="21" t="s">
+      <c r="A150" s="16"/>
+      <c r="B150" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="C150" s="21" t="s">
+      <c r="C150" s="12" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="151" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A151" s="23"/>
-      <c r="B151" s="21" t="s">
+      <c r="A151" s="16"/>
+      <c r="B151" s="12" t="s">
         <v>181</v>
       </c>
-      <c r="C151" s="21" t="s">
+      <c r="C151" s="12" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="152" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A152" s="23"/>
-      <c r="B152" s="21" t="s">
+      <c r="A152" s="16"/>
+      <c r="B152" s="12" t="s">
         <v>182</v>
       </c>
-      <c r="C152" s="21" t="s">
+      <c r="C152" s="12" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="153" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A153" s="23"/>
-      <c r="B153" s="21" t="s">
+      <c r="A153" s="16"/>
+      <c r="B153" s="12" t="s">
         <v>183</v>
       </c>
-      <c r="C153" s="21" t="s">
+      <c r="C153" s="12" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="154" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A154" s="23"/>
-      <c r="B154" s="21" t="s">
+      <c r="A154" s="16"/>
+      <c r="B154" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="C154" s="21" t="s">
+      <c r="C154" s="12" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="155" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A155" s="23"/>
-      <c r="B155" s="21" t="s">
+      <c r="A155" s="16"/>
+      <c r="B155" s="12" t="s">
         <v>185</v>
       </c>
-      <c r="C155" s="21" t="s">
+      <c r="C155" s="12" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="156" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A156" s="23"/>
-      <c r="B156" s="21" t="s">
+      <c r="A156" s="16"/>
+      <c r="B156" s="12" t="s">
         <v>186</v>
       </c>
-      <c r="C156" s="21" t="s">
+      <c r="C156" s="12" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="157" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A157" s="23"/>
-      <c r="B157" s="21" t="s">
+      <c r="A157" s="16"/>
+      <c r="B157" s="12" t="s">
         <v>187</v>
       </c>
-      <c r="C157" s="21" t="s">
+      <c r="C157" s="12" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="158" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A158" s="23"/>
-      <c r="B158" s="21" t="s">
+      <c r="A158" s="16"/>
+      <c r="B158" s="12" t="s">
         <v>188</v>
       </c>
-      <c r="C158" s="21" t="s">
+      <c r="C158" s="12" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="159" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A159" s="23"/>
-      <c r="B159" s="21" t="s">
+      <c r="A159" s="16"/>
+      <c r="B159" s="12" t="s">
         <v>189</v>
       </c>
-      <c r="C159" s="21" t="s">
+      <c r="C159" s="12" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="160" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A160" s="23"/>
-      <c r="B160" s="21" t="s">
+      <c r="A160" s="16"/>
+      <c r="B160" s="12" t="s">
         <v>190</v>
       </c>
-      <c r="C160" s="21" t="s">
+      <c r="C160" s="12" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="161" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A161" s="23"/>
-      <c r="B161" s="21" t="s">
+      <c r="A161" s="16"/>
+      <c r="B161" s="12" t="s">
         <v>191</v>
       </c>
-      <c r="C161" s="21" t="s">
+      <c r="C161" s="12" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="162" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A162" s="23"/>
-      <c r="B162" s="21" t="s">
+      <c r="A162" s="16"/>
+      <c r="B162" s="12" t="s">
         <v>192</v>
       </c>
-      <c r="C162" s="21" t="s">
+      <c r="C162" s="12" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="163" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A163" s="23"/>
-      <c r="B163" s="21" t="s">
+      <c r="A163" s="16"/>
+      <c r="B163" s="12" t="s">
         <v>193</v>
       </c>
-      <c r="C163" s="21" t="s">
+      <c r="C163" s="12" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="164" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A164" s="23"/>
-      <c r="B164" s="21" t="s">
+      <c r="A164" s="16"/>
+      <c r="B164" s="12" t="s">
         <v>194</v>
       </c>
-      <c r="C164" s="21" t="s">
+      <c r="C164" s="12" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="165" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A165" s="23"/>
-      <c r="B165" s="21" t="s">
+      <c r="A165" s="16"/>
+      <c r="B165" s="12" t="s">
         <v>195</v>
       </c>
-      <c r="C165" s="21" t="s">
+      <c r="C165" s="12" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="166" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A166" s="23"/>
-      <c r="B166" s="21" t="s">
+      <c r="A166" s="16"/>
+      <c r="B166" s="12" t="s">
         <v>196</v>
       </c>
-      <c r="C166" s="21" t="s">
+      <c r="C166" s="12" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="167" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A167" s="23"/>
-      <c r="B167" s="21" t="s">
+      <c r="A167" s="16"/>
+      <c r="B167" s="12" t="s">
         <v>197</v>
       </c>
-      <c r="C167" s="21" t="s">
+      <c r="C167" s="12" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="168" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A168" s="23"/>
-      <c r="B168" s="21" t="s">
+      <c r="A168" s="16"/>
+      <c r="B168" s="12" t="s">
         <v>198</v>
       </c>
-      <c r="C168" s="21" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="169" spans="1:3" s="25" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A169" s="26"/>
-      <c r="B169" s="24" t="s">
+      <c r="C168" s="12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" s="14" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A169" s="17"/>
+      <c r="B169" s="13" t="s">
         <v>199</v>
       </c>
-      <c r="C169" s="24" t="s">
+      <c r="C169" s="13" t="s">
         <v>65</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update upload resources files
</commit_message>
<xml_diff>
--- a/public/UploadResources/HLA_COVID19_data_dictionary.xlsx
+++ b/public/UploadResources/HLA_COVID19_data_dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arenschen/ucsf_dev_repos/hlacovid_rails/hlacovid19/public/UploadResources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55FD8CAE-3C9F-754A-95EC-F4B0944104FF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55154C44-4C07-7645-9840-D56F129028C0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2040" yWindow="460" windowWidth="20220" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_C19_DB_SUBMISSION" localSheetId="0">Sheet1!$A$3:$EK$3</definedName>
-    <definedName name="comorbs5" localSheetId="0">Sheet1!$B$140:$C$169</definedName>
+    <definedName name="_C19_DB_SUBMISSION" localSheetId="0">Sheet1!$A$4:$EK$4</definedName>
+    <definedName name="comorbs5" localSheetId="0">Sheet1!$B$141:$C$170</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="202">
   <si>
     <t>column name</t>
   </si>
@@ -640,6 +640,9 @@
   </si>
   <si>
     <t>Comorbidities</t>
+  </si>
+  <si>
+    <t>project_name</t>
   </si>
 </sst>
 </file>
@@ -833,7 +836,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -881,6 +884,10 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1100,10 +1107,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z999"/>
+  <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="G174" sqref="G174"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1148,21 +1155,22 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="19"/>
-      <c r="B3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="6" t="s">
+      <c r="A3" s="27"/>
+      <c r="B3" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="28" t="s">
         <v>7</v>
       </c>
+      <c r="E3" s="6"/>
     </row>
     <row r="4" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="19"/>
       <c r="B4" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>6</v>
@@ -1174,19 +1182,19 @@
     <row r="5" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="19"/>
       <c r="B5" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="19"/>
       <c r="B6" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>6</v>
@@ -1198,34 +1206,31 @@
     <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="19"/>
       <c r="B7" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="19"/>
-      <c r="B8" s="6" t="s">
-        <v>16</v>
+      <c r="B8" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>7</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="19"/>
       <c r="B9" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>6</v>
@@ -1234,19 +1239,19 @@
         <v>7</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="19"/>
       <c r="B10" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>19</v>
@@ -1255,83 +1260,86 @@
     <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="19"/>
       <c r="B11" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>12</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="19"/>
       <c r="B12" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="19"/>
+      <c r="B13" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C13" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="20"/>
-      <c r="B13" s="7" t="s">
+      <c r="D13" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="20"/>
+      <c r="B14" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C14" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-    </row>
-    <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="23" t="s">
+      <c r="D14" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+    </row>
+    <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B15" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="6"/>
-    </row>
-    <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="19"/>
-      <c r="B15" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>12</v>
       </c>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
     </row>
     <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="19"/>
       <c r="B16" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>6</v>
@@ -1343,7 +1351,7 @@
     <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="19"/>
       <c r="B17" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>6</v>
@@ -1355,7 +1363,7 @@
     <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="19"/>
       <c r="B18" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>6</v>
@@ -1367,7 +1375,7 @@
     <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="19"/>
       <c r="B19" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C19" s="8" t="s">
         <v>6</v>
@@ -1379,7 +1387,7 @@
     <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="19"/>
       <c r="B20" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C20" s="8" t="s">
         <v>6</v>
@@ -1391,7 +1399,7 @@
     <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="19"/>
       <c r="B21" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C21" s="8" t="s">
         <v>6</v>
@@ -1403,7 +1411,7 @@
     <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="19"/>
       <c r="B22" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C22" s="8" t="s">
         <v>6</v>
@@ -1415,7 +1423,7 @@
     <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="19"/>
       <c r="B23" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C23" s="8" t="s">
         <v>6</v>
@@ -1427,7 +1435,7 @@
     <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="19"/>
       <c r="B24" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C24" s="8" t="s">
         <v>6</v>
@@ -1439,7 +1447,7 @@
     <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="19"/>
       <c r="B25" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C25" s="8" t="s">
         <v>6</v>
@@ -1451,7 +1459,7 @@
     <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="19"/>
       <c r="B26" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>6</v>
@@ -1463,7 +1471,7 @@
     <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="19"/>
       <c r="B27" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C27" s="8" t="s">
         <v>6</v>
@@ -1475,7 +1483,7 @@
     <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="19"/>
       <c r="B28" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C28" s="8" t="s">
         <v>6</v>
@@ -1487,7 +1495,7 @@
     <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="19"/>
       <c r="B29" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C29" s="8" t="s">
         <v>6</v>
@@ -1499,22 +1507,19 @@
     <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="19"/>
       <c r="B30" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C30" s="8" t="s">
         <v>6</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="19"/>
       <c r="B31" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C31" s="8" t="s">
         <v>6</v>
@@ -1523,13 +1528,13 @@
         <v>42</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="19"/>
       <c r="B32" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C32" s="8" t="s">
         <v>6</v>
@@ -1538,13 +1543,13 @@
         <v>42</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="33" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="19"/>
       <c r="B33" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C33" s="8" t="s">
         <v>6</v>
@@ -1553,28 +1558,28 @@
         <v>42</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="34" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="19"/>
       <c r="B34" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C34" s="8" t="s">
         <v>6</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="35" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="19"/>
       <c r="B35" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C35" s="8" t="s">
         <v>6</v>
@@ -1583,13 +1588,13 @@
         <v>51</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="36" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="19"/>
       <c r="B36" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C36" s="8" t="s">
         <v>6</v>
@@ -1598,13 +1603,13 @@
         <v>51</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="37" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="19"/>
       <c r="B37" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C37" s="8" t="s">
         <v>6</v>
@@ -1613,90 +1618,93 @@
         <v>51</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="38" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="19"/>
       <c r="B38" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="39" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="19"/>
+      <c r="B39" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C38" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D38" s="6" t="s">
+      <c r="C39" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="E38" s="6" t="s">
+      <c r="E39" s="6" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="39" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="20"/>
-      <c r="B39" s="9" t="s">
+    <row r="40" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="20"/>
+      <c r="B40" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="C39" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D39" s="7" t="s">
+      <c r="C40" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="E39" s="7" t="s">
+      <c r="E40" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="F39" s="9"/>
-      <c r="G39" s="9"/>
-      <c r="H39" s="9"/>
-      <c r="I39" s="9"/>
-      <c r="J39" s="9"/>
-      <c r="K39" s="9"/>
-      <c r="L39" s="9"/>
-      <c r="M39" s="9"/>
-      <c r="N39" s="9"/>
-      <c r="O39" s="9"/>
-      <c r="P39" s="9"/>
-      <c r="Q39" s="9"/>
-      <c r="R39" s="9"/>
-      <c r="S39" s="9"/>
-      <c r="T39" s="9"/>
-      <c r="U39" s="9"/>
-      <c r="V39" s="9"/>
-      <c r="W39" s="9"/>
-      <c r="X39" s="9"/>
-      <c r="Y39" s="9"/>
-      <c r="Z39" s="9"/>
-    </row>
-    <row r="40" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="24" t="s">
+      <c r="F40" s="9"/>
+      <c r="G40" s="9"/>
+      <c r="H40" s="9"/>
+      <c r="I40" s="9"/>
+      <c r="J40" s="9"/>
+      <c r="K40" s="9"/>
+      <c r="L40" s="9"/>
+      <c r="M40" s="9"/>
+      <c r="N40" s="9"/>
+      <c r="O40" s="9"/>
+      <c r="P40" s="9"/>
+      <c r="Q40" s="9"/>
+      <c r="R40" s="9"/>
+      <c r="S40" s="9"/>
+      <c r="T40" s="9"/>
+      <c r="U40" s="9"/>
+      <c r="V40" s="9"/>
+      <c r="W40" s="9"/>
+      <c r="X40" s="9"/>
+      <c r="Y40" s="9"/>
+      <c r="Z40" s="9"/>
+    </row>
+    <row r="41" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="B40" s="6" t="s">
+      <c r="B41" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="C40" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="D40" s="6" t="s">
+      <c r="C41" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="D41" s="6" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="41" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="19"/>
-      <c r="B41" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C41" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="D41" s="6" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="42" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="19"/>
-      <c r="B42" s="5" t="s">
-        <v>67</v>
+      <c r="B42" s="6" t="s">
+        <v>66</v>
       </c>
       <c r="C42" s="8" t="s">
         <v>65</v>
@@ -1708,7 +1716,7 @@
     <row r="43" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="19"/>
       <c r="B43" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C43" s="8" t="s">
         <v>65</v>
@@ -1720,10 +1728,10 @@
     <row r="44" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="19"/>
       <c r="B44" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="D44" s="6" t="s">
         <v>12</v>
@@ -1732,10 +1740,10 @@
     <row r="45" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="19"/>
       <c r="B45" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>65</v>
+        <v>15</v>
       </c>
       <c r="D45" s="6" t="s">
         <v>12</v>
@@ -1744,7 +1752,7 @@
     <row r="46" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="19"/>
       <c r="B46" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C46" s="8" t="s">
         <v>65</v>
@@ -1756,10 +1764,10 @@
     <row r="47" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="19"/>
       <c r="B47" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="D47" s="6" t="s">
         <v>12</v>
@@ -1768,7 +1776,7 @@
     <row r="48" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="19"/>
       <c r="B48" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C48" s="8" t="s">
         <v>15</v>
@@ -1780,10 +1788,10 @@
     <row r="49" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="19"/>
       <c r="B49" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>65</v>
+        <v>15</v>
       </c>
       <c r="D49" s="6" t="s">
         <v>12</v>
@@ -1792,7 +1800,7 @@
     <row r="50" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="19"/>
       <c r="B50" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C50" s="8" t="s">
         <v>65</v>
@@ -1804,7 +1812,7 @@
     <row r="51" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="19"/>
       <c r="B51" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C51" s="8" t="s">
         <v>65</v>
@@ -1816,7 +1824,7 @@
     <row r="52" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="19"/>
       <c r="B52" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C52" s="8" t="s">
         <v>65</v>
@@ -1828,7 +1836,7 @@
     <row r="53" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="19"/>
       <c r="B53" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C53" s="8" t="s">
         <v>65</v>
@@ -1840,7 +1848,7 @@
     <row r="54" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="19"/>
       <c r="B54" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C54" s="8" t="s">
         <v>65</v>
@@ -1852,7 +1860,7 @@
     <row r="55" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="19"/>
       <c r="B55" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C55" s="8" t="s">
         <v>65</v>
@@ -1864,70 +1872,70 @@
     <row r="56" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="19"/>
       <c r="B56" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C56" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="D56" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="57" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="19"/>
+      <c r="B57" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="C56" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="D56" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="57" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="20"/>
-      <c r="B57" s="9" t="s">
+      <c r="C57" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="D57" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="58" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="20"/>
+      <c r="B58" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="C57" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D57" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E57" s="9"/>
-      <c r="F57" s="9"/>
-      <c r="G57" s="9"/>
-      <c r="H57" s="9"/>
-      <c r="I57" s="9"/>
-      <c r="J57" s="9"/>
-      <c r="K57" s="9"/>
-      <c r="L57" s="9"/>
-      <c r="M57" s="9"/>
-      <c r="N57" s="9"/>
-      <c r="O57" s="9"/>
-      <c r="P57" s="9"/>
-      <c r="Q57" s="9"/>
-      <c r="R57" s="9"/>
-      <c r="S57" s="9"/>
-      <c r="T57" s="9"/>
-      <c r="U57" s="9"/>
-      <c r="V57" s="9"/>
-      <c r="W57" s="9"/>
-      <c r="X57" s="9"/>
-      <c r="Y57" s="9"/>
-      <c r="Z57" s="9"/>
-    </row>
-    <row r="58" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="25" t="s">
+      <c r="C58" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D58" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E58" s="9"/>
+      <c r="F58" s="9"/>
+      <c r="G58" s="9"/>
+      <c r="H58" s="9"/>
+      <c r="I58" s="9"/>
+      <c r="J58" s="9"/>
+      <c r="K58" s="9"/>
+      <c r="L58" s="9"/>
+      <c r="M58" s="9"/>
+      <c r="N58" s="9"/>
+      <c r="O58" s="9"/>
+      <c r="P58" s="9"/>
+      <c r="Q58" s="9"/>
+      <c r="R58" s="9"/>
+      <c r="S58" s="9"/>
+      <c r="T58" s="9"/>
+      <c r="U58" s="9"/>
+      <c r="V58" s="9"/>
+      <c r="W58" s="9"/>
+      <c r="X58" s="9"/>
+      <c r="Y58" s="9"/>
+      <c r="Z58" s="9"/>
+    </row>
+    <row r="59" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="25" t="s">
         <v>83</v>
       </c>
-      <c r="B58" s="5" t="s">
+      <c r="B59" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="C58" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="D58" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="59" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="19"/>
-      <c r="B59" s="5" t="s">
-        <v>85</v>
-      </c>
       <c r="C59" s="8" t="s">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="D59" s="6" t="s">
         <v>12</v>
@@ -1935,11 +1943,11 @@
     </row>
     <row r="60" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="19"/>
-      <c r="B60" s="6" t="s">
-        <v>86</v>
+      <c r="B60" s="5" t="s">
+        <v>85</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>65</v>
+        <v>15</v>
       </c>
       <c r="D60" s="6" t="s">
         <v>12</v>
@@ -1947,11 +1955,11 @@
     </row>
     <row r="61" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="19"/>
-      <c r="B61" s="5" t="s">
-        <v>87</v>
+      <c r="B61" s="6" t="s">
+        <v>86</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="D61" s="6" t="s">
         <v>12</v>
@@ -1960,10 +1968,10 @@
     <row r="62" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="19"/>
       <c r="B62" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C62" s="8" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D62" s="6" t="s">
         <v>12</v>
@@ -1972,10 +1980,10 @@
     <row r="63" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="19"/>
       <c r="B63" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C63" s="8" t="s">
-        <v>65</v>
+        <v>6</v>
       </c>
       <c r="D63" s="6" t="s">
         <v>12</v>
@@ -1984,10 +1992,10 @@
     <row r="64" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="19"/>
       <c r="B64" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C64" s="8" t="s">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="D64" s="6" t="s">
         <v>12</v>
@@ -1996,10 +2004,10 @@
     <row r="65" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="19"/>
       <c r="B65" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>65</v>
+        <v>15</v>
       </c>
       <c r="D65" s="6" t="s">
         <v>12</v>
@@ -2008,7 +2016,7 @@
     <row r="66" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="19"/>
       <c r="B66" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C66" s="8" t="s">
         <v>65</v>
@@ -2020,10 +2028,10 @@
     <row r="67" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="19"/>
       <c r="B67" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C67" s="8" t="s">
-        <v>6</v>
+        <v>65</v>
       </c>
       <c r="D67" s="6" t="s">
         <v>12</v>
@@ -2032,10 +2040,10 @@
     <row r="68" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="19"/>
       <c r="B68" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C68" s="8" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D68" s="6" t="s">
         <v>12</v>
@@ -2044,7 +2052,7 @@
     <row r="69" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="19"/>
       <c r="B69" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C69" s="8" t="s">
         <v>15</v>
@@ -2056,10 +2064,10 @@
     <row r="70" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="19"/>
       <c r="B70" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C70" s="8" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D70" s="6" t="s">
         <v>12</v>
@@ -2068,10 +2076,10 @@
     <row r="71" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="19"/>
       <c r="B71" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C71" s="8" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D71" s="6" t="s">
         <v>12</v>
@@ -2080,7 +2088,7 @@
     <row r="72" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="19"/>
       <c r="B72" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C72" s="8" t="s">
         <v>15</v>
@@ -2092,7 +2100,7 @@
     <row r="73" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="19"/>
       <c r="B73" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C73" s="8" t="s">
         <v>15</v>
@@ -2104,7 +2112,7 @@
     <row r="74" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="19"/>
       <c r="B74" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C74" s="8" t="s">
         <v>15</v>
@@ -2116,10 +2124,10 @@
     <row r="75" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="19"/>
       <c r="B75" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C75" s="8" t="s">
-        <v>65</v>
+        <v>15</v>
       </c>
       <c r="D75" s="6" t="s">
         <v>12</v>
@@ -2128,10 +2136,10 @@
     <row r="76" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="19"/>
       <c r="B76" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C76" s="8" t="s">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="D76" s="6" t="s">
         <v>12</v>
@@ -2140,7 +2148,7 @@
     <row r="77" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="19"/>
       <c r="B77" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C77" s="8" t="s">
         <v>15</v>
@@ -2152,10 +2160,10 @@
     <row r="78" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="19"/>
       <c r="B78" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C78" s="8" t="s">
-        <v>65</v>
+        <v>15</v>
       </c>
       <c r="D78" s="6" t="s">
         <v>12</v>
@@ -2164,7 +2172,7 @@
     <row r="79" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="19"/>
       <c r="B79" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C79" s="8" t="s">
         <v>65</v>
@@ -2176,7 +2184,7 @@
     <row r="80" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="19"/>
       <c r="B80" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C80" s="8" t="s">
         <v>65</v>
@@ -2188,7 +2196,7 @@
     <row r="81" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="19"/>
       <c r="B81" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C81" s="8" t="s">
         <v>65</v>
@@ -2200,7 +2208,7 @@
     <row r="82" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="19"/>
       <c r="B82" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C82" s="8" t="s">
         <v>65</v>
@@ -2212,70 +2220,70 @@
     <row r="83" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="19"/>
       <c r="B83" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C83" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="D83" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="84" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="19"/>
+      <c r="B84" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="C83" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="D83" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="84" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="20"/>
-      <c r="B84" s="9" t="s">
+      <c r="C84" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="D84" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="85" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="20"/>
+      <c r="B85" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="C84" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="D84" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E84" s="9"/>
-      <c r="F84" s="9"/>
-      <c r="G84" s="9"/>
-      <c r="H84" s="9"/>
-      <c r="I84" s="9"/>
-      <c r="J84" s="9"/>
-      <c r="K84" s="9"/>
-      <c r="L84" s="9"/>
-      <c r="M84" s="9"/>
-      <c r="N84" s="9"/>
-      <c r="O84" s="9"/>
-      <c r="P84" s="9"/>
-      <c r="Q84" s="9"/>
-      <c r="R84" s="9"/>
-      <c r="S84" s="9"/>
-      <c r="T84" s="9"/>
-      <c r="U84" s="9"/>
-      <c r="V84" s="9"/>
-      <c r="W84" s="9"/>
-      <c r="X84" s="9"/>
-      <c r="Y84" s="9"/>
-      <c r="Z84" s="9"/>
-    </row>
-    <row r="85" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="26" t="s">
+      <c r="C85" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="D85" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E85" s="9"/>
+      <c r="F85" s="9"/>
+      <c r="G85" s="9"/>
+      <c r="H85" s="9"/>
+      <c r="I85" s="9"/>
+      <c r="J85" s="9"/>
+      <c r="K85" s="9"/>
+      <c r="L85" s="9"/>
+      <c r="M85" s="9"/>
+      <c r="N85" s="9"/>
+      <c r="O85" s="9"/>
+      <c r="P85" s="9"/>
+      <c r="Q85" s="9"/>
+      <c r="R85" s="9"/>
+      <c r="S85" s="9"/>
+      <c r="T85" s="9"/>
+      <c r="U85" s="9"/>
+      <c r="V85" s="9"/>
+      <c r="W85" s="9"/>
+      <c r="X85" s="9"/>
+      <c r="Y85" s="9"/>
+      <c r="Z85" s="9"/>
+    </row>
+    <row r="86" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="26" t="s">
         <v>111</v>
       </c>
-      <c r="B85" s="6" t="s">
+      <c r="B86" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="C85" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="D85" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="86" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="19"/>
-      <c r="B86" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="C86" s="8" t="s">
-        <v>6</v>
+      <c r="C86" s="10" t="s">
+        <v>65</v>
       </c>
       <c r="D86" s="6" t="s">
         <v>12</v>
@@ -2284,67 +2292,67 @@
     <row r="87" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="19"/>
       <c r="B87" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C87" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D87" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="88" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="19"/>
+      <c r="B88" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="C87" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D87" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="88" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="20"/>
-      <c r="B88" s="9" t="s">
+      <c r="C88" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D88" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="89" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A89" s="20"/>
+      <c r="B89" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="C88" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D88" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E88" s="9"/>
-      <c r="F88" s="9"/>
-      <c r="G88" s="9"/>
-      <c r="H88" s="9"/>
-      <c r="I88" s="9"/>
-      <c r="J88" s="9"/>
-      <c r="K88" s="9"/>
-      <c r="L88" s="9"/>
-      <c r="M88" s="9"/>
-      <c r="N88" s="9"/>
-      <c r="O88" s="9"/>
-      <c r="P88" s="9"/>
-      <c r="Q88" s="9"/>
-      <c r="R88" s="9"/>
-      <c r="S88" s="9"/>
-      <c r="T88" s="9"/>
-      <c r="U88" s="9"/>
-      <c r="V88" s="9"/>
-      <c r="W88" s="9"/>
-      <c r="X88" s="9"/>
-      <c r="Y88" s="9"/>
-      <c r="Z88" s="9"/>
-    </row>
-    <row r="89" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="18" t="s">
+      <c r="C89" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D89" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E89" s="9"/>
+      <c r="F89" s="9"/>
+      <c r="G89" s="9"/>
+      <c r="H89" s="9"/>
+      <c r="I89" s="9"/>
+      <c r="J89" s="9"/>
+      <c r="K89" s="9"/>
+      <c r="L89" s="9"/>
+      <c r="M89" s="9"/>
+      <c r="N89" s="9"/>
+      <c r="O89" s="9"/>
+      <c r="P89" s="9"/>
+      <c r="Q89" s="9"/>
+      <c r="R89" s="9"/>
+      <c r="S89" s="9"/>
+      <c r="T89" s="9"/>
+      <c r="U89" s="9"/>
+      <c r="V89" s="9"/>
+      <c r="W89" s="9"/>
+      <c r="X89" s="9"/>
+      <c r="Y89" s="9"/>
+      <c r="Z89" s="9"/>
+    </row>
+    <row r="90" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A90" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="B89" s="5" t="s">
+      <c r="B90" s="5" t="s">
         <v>117</v>
-      </c>
-      <c r="C89" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D89" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="90" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="19"/>
-      <c r="B90" s="5" t="s">
-        <v>118</v>
       </c>
       <c r="C90" s="8" t="s">
         <v>6</v>
@@ -2356,7 +2364,7 @@
     <row r="91" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="19"/>
       <c r="B91" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C91" s="8" t="s">
         <v>6</v>
@@ -2368,7 +2376,7 @@
     <row r="92" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="19"/>
       <c r="B92" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C92" s="8" t="s">
         <v>6</v>
@@ -2380,7 +2388,7 @@
     <row r="93" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="19"/>
       <c r="B93" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C93" s="8" t="s">
         <v>6</v>
@@ -2392,7 +2400,7 @@
     <row r="94" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="19"/>
       <c r="B94" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C94" s="8" t="s">
         <v>6</v>
@@ -2404,7 +2412,7 @@
     <row r="95" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="19"/>
       <c r="B95" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C95" s="8" t="s">
         <v>6</v>
@@ -2416,7 +2424,7 @@
     <row r="96" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="19"/>
       <c r="B96" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C96" s="8" t="s">
         <v>6</v>
@@ -2428,7 +2436,7 @@
     <row r="97" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="19"/>
       <c r="B97" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C97" s="8" t="s">
         <v>6</v>
@@ -2440,7 +2448,7 @@
     <row r="98" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="19"/>
       <c r="B98" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C98" s="8" t="s">
         <v>6</v>
@@ -2452,7 +2460,7 @@
     <row r="99" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="19"/>
       <c r="B99" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C99" s="8" t="s">
         <v>6</v>
@@ -2464,7 +2472,7 @@
     <row r="100" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="19"/>
       <c r="B100" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C100" s="8" t="s">
         <v>6</v>
@@ -2476,7 +2484,7 @@
     <row r="101" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="19"/>
       <c r="B101" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C101" s="8" t="s">
         <v>6</v>
@@ -2488,7 +2496,7 @@
     <row r="102" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="19"/>
       <c r="B102" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C102" s="8" t="s">
         <v>6</v>
@@ -2500,7 +2508,7 @@
     <row r="103" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="19"/>
       <c r="B103" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C103" s="8" t="s">
         <v>6</v>
@@ -2512,7 +2520,7 @@
     <row r="104" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="19"/>
       <c r="B104" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C104" s="8" t="s">
         <v>6</v>
@@ -2524,7 +2532,7 @@
     <row r="105" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="19"/>
       <c r="B105" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C105" s="8" t="s">
         <v>6</v>
@@ -2536,7 +2544,7 @@
     <row r="106" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="19"/>
       <c r="B106" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C106" s="8" t="s">
         <v>6</v>
@@ -2548,7 +2556,7 @@
     <row r="107" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="19"/>
       <c r="B107" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C107" s="8" t="s">
         <v>6</v>
@@ -2560,7 +2568,7 @@
     <row r="108" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="19"/>
       <c r="B108" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C108" s="8" t="s">
         <v>6</v>
@@ -2572,7 +2580,7 @@
     <row r="109" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="19"/>
       <c r="B109" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C109" s="8" t="s">
         <v>6</v>
@@ -2584,7 +2592,7 @@
     <row r="110" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="19"/>
       <c r="B110" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C110" s="8" t="s">
         <v>6</v>
@@ -2596,7 +2604,7 @@
     <row r="111" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="19"/>
       <c r="B111" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C111" s="8" t="s">
         <v>6</v>
@@ -2608,7 +2616,7 @@
     <row r="112" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="19"/>
       <c r="B112" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C112" s="8" t="s">
         <v>6</v>
@@ -2620,7 +2628,7 @@
     <row r="113" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="19"/>
       <c r="B113" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C113" s="8" t="s">
         <v>6</v>
@@ -2632,7 +2640,7 @@
     <row r="114" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="19"/>
       <c r="B114" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C114" s="8" t="s">
         <v>6</v>
@@ -2644,7 +2652,7 @@
     <row r="115" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="19"/>
       <c r="B115" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C115" s="8" t="s">
         <v>6</v>
@@ -2656,7 +2664,7 @@
     <row r="116" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="19"/>
       <c r="B116" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C116" s="8" t="s">
         <v>6</v>
@@ -2668,7 +2676,7 @@
     <row r="117" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="19"/>
       <c r="B117" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C117" s="8" t="s">
         <v>6</v>
@@ -2680,7 +2688,7 @@
     <row r="118" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="19"/>
       <c r="B118" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C118" s="8" t="s">
         <v>6</v>
@@ -2692,7 +2700,7 @@
     <row r="119" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="19"/>
       <c r="B119" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C119" s="8" t="s">
         <v>6</v>
@@ -2704,7 +2712,7 @@
     <row r="120" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="19"/>
       <c r="B120" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C120" s="8" t="s">
         <v>6</v>
@@ -2716,70 +2724,70 @@
     <row r="121" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="19"/>
       <c r="B121" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="C121" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D121" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="122" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A122" s="19"/>
+      <c r="B122" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="C121" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D121" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="122" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A122" s="20"/>
-      <c r="B122" s="9" t="s">
+      <c r="C122" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D122" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="123" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A123" s="20"/>
+      <c r="B123" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="C122" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D122" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E122" s="9"/>
-      <c r="F122" s="9"/>
-      <c r="G122" s="9"/>
-      <c r="H122" s="9"/>
-      <c r="I122" s="9"/>
-      <c r="J122" s="9"/>
-      <c r="K122" s="9"/>
-      <c r="L122" s="9"/>
-      <c r="M122" s="9"/>
-      <c r="N122" s="9"/>
-      <c r="O122" s="9"/>
-      <c r="P122" s="9"/>
-      <c r="Q122" s="9"/>
-      <c r="R122" s="9"/>
-      <c r="S122" s="9"/>
-      <c r="T122" s="9"/>
-      <c r="U122" s="9"/>
-      <c r="V122" s="9"/>
-      <c r="W122" s="9"/>
-      <c r="X122" s="9"/>
-      <c r="Y122" s="9"/>
-      <c r="Z122" s="9"/>
-    </row>
-    <row r="123" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A123" s="21" t="s">
+      <c r="C123" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D123" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E123" s="9"/>
+      <c r="F123" s="9"/>
+      <c r="G123" s="9"/>
+      <c r="H123" s="9"/>
+      <c r="I123" s="9"/>
+      <c r="J123" s="9"/>
+      <c r="K123" s="9"/>
+      <c r="L123" s="9"/>
+      <c r="M123" s="9"/>
+      <c r="N123" s="9"/>
+      <c r="O123" s="9"/>
+      <c r="P123" s="9"/>
+      <c r="Q123" s="9"/>
+      <c r="R123" s="9"/>
+      <c r="S123" s="9"/>
+      <c r="T123" s="9"/>
+      <c r="U123" s="9"/>
+      <c r="V123" s="9"/>
+      <c r="W123" s="9"/>
+      <c r="X123" s="9"/>
+      <c r="Y123" s="9"/>
+      <c r="Z123" s="9"/>
+    </row>
+    <row r="124" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A124" s="21" t="s">
         <v>151</v>
       </c>
-      <c r="B123" s="5" t="s">
+      <c r="B124" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="C123" s="8" t="s">
+      <c r="C124" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="D123" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="124" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A124" s="19"/>
-      <c r="B124" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="C124" s="8" t="s">
-        <v>6</v>
       </c>
       <c r="D124" s="6" t="s">
         <v>12</v>
@@ -2788,7 +2796,7 @@
     <row r="125" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="19"/>
       <c r="B125" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C125" s="8" t="s">
         <v>6</v>
@@ -2800,7 +2808,7 @@
     <row r="126" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="19"/>
       <c r="B126" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C126" s="8" t="s">
         <v>6</v>
@@ -2812,7 +2820,7 @@
     <row r="127" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="19"/>
       <c r="B127" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C127" s="8" t="s">
         <v>6</v>
@@ -2824,7 +2832,7 @@
     <row r="128" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="19"/>
       <c r="B128" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C128" s="8" t="s">
         <v>6</v>
@@ -2836,7 +2844,7 @@
     <row r="129" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="19"/>
       <c r="B129" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C129" s="8" t="s">
         <v>6</v>
@@ -2848,7 +2856,7 @@
     <row r="130" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="19"/>
       <c r="B130" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C130" s="8" t="s">
         <v>6</v>
@@ -2860,7 +2868,7 @@
     <row r="131" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="19"/>
       <c r="B131" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C131" s="8" t="s">
         <v>6</v>
@@ -2872,7 +2880,7 @@
     <row r="132" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="19"/>
       <c r="B132" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C132" s="8" t="s">
         <v>6</v>
@@ -2884,7 +2892,7 @@
     <row r="133" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="19"/>
       <c r="B133" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C133" s="8" t="s">
         <v>6</v>
@@ -2896,7 +2904,7 @@
     <row r="134" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="19"/>
       <c r="B134" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C134" s="8" t="s">
         <v>6</v>
@@ -2908,7 +2916,7 @@
     <row r="135" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="19"/>
       <c r="B135" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C135" s="8" t="s">
         <v>6</v>
@@ -2920,7 +2928,7 @@
     <row r="136" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="19"/>
       <c r="B136" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C136" s="8" t="s">
         <v>6</v>
@@ -2932,7 +2940,7 @@
     <row r="137" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="19"/>
       <c r="B137" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C137" s="8" t="s">
         <v>6</v>
@@ -2944,73 +2952,76 @@
     <row r="138" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" s="19"/>
       <c r="B138" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="C138" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D138" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="139" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A139" s="19"/>
+      <c r="B139" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="C138" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D138" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="139" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A139" s="20"/>
-      <c r="B139" s="9" t="s">
+      <c r="C139" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D139" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="140" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A140" s="20"/>
+      <c r="B140" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="C139" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D139" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E139" s="9"/>
-      <c r="F139" s="9"/>
-      <c r="G139" s="9"/>
-      <c r="H139" s="9"/>
-      <c r="I139" s="9"/>
-      <c r="J139" s="9"/>
-      <c r="K139" s="9"/>
-      <c r="L139" s="9"/>
-      <c r="M139" s="9"/>
-      <c r="N139" s="9"/>
-      <c r="O139" s="9"/>
-      <c r="P139" s="9"/>
-      <c r="Q139" s="9"/>
-      <c r="R139" s="9"/>
-      <c r="S139" s="9"/>
-      <c r="T139" s="9"/>
-      <c r="U139" s="9"/>
-      <c r="V139" s="9"/>
-      <c r="W139" s="9"/>
-      <c r="X139" s="9"/>
-      <c r="Y139" s="9"/>
-      <c r="Z139" s="9"/>
-    </row>
-    <row r="140" spans="1:26" ht="16" x14ac:dyDescent="0.2">
-      <c r="A140" s="15" t="s">
+      <c r="C140" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D140" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E140" s="9"/>
+      <c r="F140" s="9"/>
+      <c r="G140" s="9"/>
+      <c r="H140" s="9"/>
+      <c r="I140" s="9"/>
+      <c r="J140" s="9"/>
+      <c r="K140" s="9"/>
+      <c r="L140" s="9"/>
+      <c r="M140" s="9"/>
+      <c r="N140" s="9"/>
+      <c r="O140" s="9"/>
+      <c r="P140" s="9"/>
+      <c r="Q140" s="9"/>
+      <c r="R140" s="9"/>
+      <c r="S140" s="9"/>
+      <c r="T140" s="9"/>
+      <c r="U140" s="9"/>
+      <c r="V140" s="9"/>
+      <c r="W140" s="9"/>
+      <c r="X140" s="9"/>
+      <c r="Y140" s="9"/>
+      <c r="Z140" s="9"/>
+    </row>
+    <row r="141" spans="1:26" ht="16" x14ac:dyDescent="0.2">
+      <c r="A141" s="15" t="s">
         <v>200</v>
       </c>
-      <c r="B140" s="12" t="s">
+      <c r="B141" s="12" t="s">
         <v>169</v>
       </c>
-      <c r="C140" s="12" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="141" spans="1:26" ht="16" x14ac:dyDescent="0.2">
-      <c r="A141" s="16"/>
-      <c r="B141" s="12" t="s">
-        <v>170</v>
-      </c>
       <c r="C141" s="12" t="s">
-        <v>171</v>
+        <v>65</v>
       </c>
     </row>
     <row r="142" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A142" s="16"/>
       <c r="B142" s="12" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C142" s="12" t="s">
         <v>171</v>
@@ -3019,16 +3030,16 @@
     <row r="143" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A143" s="16"/>
       <c r="B143" s="12" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C143" s="12" t="s">
-        <v>65</v>
+        <v>171</v>
       </c>
     </row>
     <row r="144" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A144" s="16"/>
       <c r="B144" s="12" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C144" s="12" t="s">
         <v>65</v>
@@ -3037,25 +3048,25 @@
     <row r="145" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A145" s="16"/>
       <c r="B145" s="12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C145" s="12" t="s">
-        <v>6</v>
+        <v>65</v>
       </c>
     </row>
     <row r="146" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A146" s="16"/>
       <c r="B146" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C146" s="12" t="s">
-        <v>65</v>
+        <v>6</v>
       </c>
     </row>
     <row r="147" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A147" s="16"/>
       <c r="B147" s="12" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C147" s="12" t="s">
         <v>65</v>
@@ -3064,7 +3075,7 @@
     <row r="148" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A148" s="16"/>
       <c r="B148" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C148" s="12" t="s">
         <v>65</v>
@@ -3073,7 +3084,7 @@
     <row r="149" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A149" s="16"/>
       <c r="B149" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C149" s="12" t="s">
         <v>65</v>
@@ -3082,7 +3093,7 @@
     <row r="150" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A150" s="16"/>
       <c r="B150" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C150" s="12" t="s">
         <v>65</v>
@@ -3091,7 +3102,7 @@
     <row r="151" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A151" s="16"/>
       <c r="B151" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C151" s="12" t="s">
         <v>65</v>
@@ -3100,7 +3111,7 @@
     <row r="152" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A152" s="16"/>
       <c r="B152" s="12" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C152" s="12" t="s">
         <v>65</v>
@@ -3109,7 +3120,7 @@
     <row r="153" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A153" s="16"/>
       <c r="B153" s="12" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C153" s="12" t="s">
         <v>65</v>
@@ -3118,7 +3129,7 @@
     <row r="154" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A154" s="16"/>
       <c r="B154" s="12" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C154" s="12" t="s">
         <v>65</v>
@@ -3127,7 +3138,7 @@
     <row r="155" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A155" s="16"/>
       <c r="B155" s="12" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C155" s="12" t="s">
         <v>65</v>
@@ -3136,7 +3147,7 @@
     <row r="156" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A156" s="16"/>
       <c r="B156" s="12" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C156" s="12" t="s">
         <v>65</v>
@@ -3145,7 +3156,7 @@
     <row r="157" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A157" s="16"/>
       <c r="B157" s="12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C157" s="12" t="s">
         <v>65</v>
@@ -3154,7 +3165,7 @@
     <row r="158" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A158" s="16"/>
       <c r="B158" s="12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C158" s="12" t="s">
         <v>65</v>
@@ -3163,7 +3174,7 @@
     <row r="159" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A159" s="16"/>
       <c r="B159" s="12" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C159" s="12" t="s">
         <v>65</v>
@@ -3172,7 +3183,7 @@
     <row r="160" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A160" s="16"/>
       <c r="B160" s="12" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C160" s="12" t="s">
         <v>65</v>
@@ -3181,7 +3192,7 @@
     <row r="161" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A161" s="16"/>
       <c r="B161" s="12" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C161" s="12" t="s">
         <v>65</v>
@@ -3190,7 +3201,7 @@
     <row r="162" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A162" s="16"/>
       <c r="B162" s="12" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C162" s="12" t="s">
         <v>65</v>
@@ -3199,7 +3210,7 @@
     <row r="163" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A163" s="16"/>
       <c r="B163" s="12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C163" s="12" t="s">
         <v>65</v>
@@ -3208,7 +3219,7 @@
     <row r="164" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A164" s="16"/>
       <c r="B164" s="12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C164" s="12" t="s">
         <v>65</v>
@@ -3217,7 +3228,7 @@
     <row r="165" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A165" s="16"/>
       <c r="B165" s="12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C165" s="12" t="s">
         <v>65</v>
@@ -3226,7 +3237,7 @@
     <row r="166" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A166" s="16"/>
       <c r="B166" s="12" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C166" s="12" t="s">
         <v>65</v>
@@ -3235,7 +3246,7 @@
     <row r="167" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A167" s="16"/>
       <c r="B167" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C167" s="12" t="s">
         <v>65</v>
@@ -3244,22 +3255,30 @@
     <row r="168" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A168" s="16"/>
       <c r="B168" s="12" t="s">
+        <v>197</v>
+      </c>
+      <c r="C168" s="12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A169" s="16"/>
+      <c r="B169" s="12" t="s">
         <v>198</v>
       </c>
-      <c r="C168" s="12" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="169" spans="1:3" s="14" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A169" s="17"/>
-      <c r="B169" s="13" t="s">
+      <c r="C169" s="12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" s="14" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A170" s="17"/>
+      <c r="B170" s="13" t="s">
         <v>199</v>
       </c>
-      <c r="C169" s="13" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="170" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="C170" s="13" t="s">
+        <v>65</v>
+      </c>
+    </row>
     <row r="171" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="172" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="173" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4089,16 +4108,17 @@
     <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="A140:A169"/>
-    <mergeCell ref="A89:A122"/>
-    <mergeCell ref="A123:A139"/>
-    <mergeCell ref="A2:A13"/>
-    <mergeCell ref="A14:A39"/>
-    <mergeCell ref="A40:A57"/>
-    <mergeCell ref="A58:A84"/>
-    <mergeCell ref="A85:A88"/>
+    <mergeCell ref="A141:A170"/>
+    <mergeCell ref="A90:A123"/>
+    <mergeCell ref="A124:A140"/>
+    <mergeCell ref="A2:A14"/>
+    <mergeCell ref="A15:A40"/>
+    <mergeCell ref="A41:A58"/>
+    <mergeCell ref="A59:A85"/>
+    <mergeCell ref="A86:A89"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>

<commit_message>
Update UploadResources download sheets
</commit_message>
<xml_diff>
--- a/public/UploadResources/HLA_COVID19_data_dictionary.xlsx
+++ b/public/UploadResources/HLA_COVID19_data_dictionary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10615"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arenschen/ucsf_dev_repos/hlacovid_rails/hlacovid19/public/UploadResources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3F82B30-6BE1-D147-B3C6-4CCD144409D1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25DE4A5A-03CB-DC4A-A5CA-ADD0E0533673}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2040" yWindow="460" windowWidth="20220" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -234,9 +234,6 @@
     <t>boolean(T/F)</t>
   </si>
   <si>
-    <t>patient_self_reported_positive</t>
-  </si>
-  <si>
     <t>dry_cough</t>
   </si>
   <si>
@@ -643,6 +640,9 @@
   </si>
   <si>
     <t>When typing_method_name is populated</t>
+  </si>
+  <si>
+    <t>type_of_c19_test</t>
   </si>
 </sst>
 </file>
@@ -1109,8 +1109,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D10" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1157,7 +1157,7 @@
     <row r="3" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="24"/>
       <c r="B3" s="8" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>6</v>
@@ -1633,7 +1633,7 @@
         <v>51</v>
       </c>
       <c r="E38" s="15" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="39" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1703,11 +1703,11 @@
     </row>
     <row r="42" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="20"/>
-      <c r="B42" s="6" t="s">
-        <v>65</v>
+      <c r="B42" s="15" t="s">
+        <v>201</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>64</v>
+        <v>6</v>
       </c>
       <c r="D42" s="6" t="s">
         <v>12</v>
@@ -1716,7 +1716,7 @@
     <row r="43" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="20"/>
       <c r="B43" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C43" s="8" t="s">
         <v>64</v>
@@ -1728,7 +1728,7 @@
     <row r="44" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="20"/>
       <c r="B44" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C44" s="8" t="s">
         <v>64</v>
@@ -1740,7 +1740,7 @@
     <row r="45" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="20"/>
       <c r="B45" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C45" s="8" t="s">
         <v>15</v>
@@ -1752,7 +1752,7 @@
     <row r="46" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="20"/>
       <c r="B46" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C46" s="8" t="s">
         <v>64</v>
@@ -1764,7 +1764,7 @@
     <row r="47" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="20"/>
       <c r="B47" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C47" s="8" t="s">
         <v>64</v>
@@ -1776,7 +1776,7 @@
     <row r="48" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="20"/>
       <c r="B48" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C48" s="8" t="s">
         <v>15</v>
@@ -1788,7 +1788,7 @@
     <row r="49" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="20"/>
       <c r="B49" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C49" s="8" t="s">
         <v>15</v>
@@ -1800,7 +1800,7 @@
     <row r="50" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="20"/>
       <c r="B50" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C50" s="8" t="s">
         <v>64</v>
@@ -1812,7 +1812,7 @@
     <row r="51" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="20"/>
       <c r="B51" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C51" s="8" t="s">
         <v>64</v>
@@ -1824,7 +1824,7 @@
     <row r="52" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="20"/>
       <c r="B52" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C52" s="8" t="s">
         <v>64</v>
@@ -1836,7 +1836,7 @@
     <row r="53" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="20"/>
       <c r="B53" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C53" s="8" t="s">
         <v>64</v>
@@ -1848,7 +1848,7 @@
     <row r="54" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="20"/>
       <c r="B54" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C54" s="8" t="s">
         <v>64</v>
@@ -1860,7 +1860,7 @@
     <row r="55" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="20"/>
       <c r="B55" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C55" s="8" t="s">
         <v>64</v>
@@ -1872,7 +1872,7 @@
     <row r="56" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="20"/>
       <c r="B56" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C56" s="8" t="s">
         <v>64</v>
@@ -1884,7 +1884,7 @@
     <row r="57" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="20"/>
       <c r="B57" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C57" s="8" t="s">
         <v>64</v>
@@ -1896,7 +1896,7 @@
     <row r="58" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="21"/>
       <c r="B58" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C58" s="9" t="s">
         <v>6</v>
@@ -1929,10 +1929,10 @@
     </row>
     <row r="59" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="B59" s="5" t="s">
         <v>82</v>
-      </c>
-      <c r="B59" s="5" t="s">
-        <v>83</v>
       </c>
       <c r="C59" s="8" t="s">
         <v>64</v>
@@ -1944,7 +1944,7 @@
     <row r="60" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="20"/>
       <c r="B60" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C60" s="8" t="s">
         <v>15</v>
@@ -1956,7 +1956,7 @@
     <row r="61" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="20"/>
       <c r="B61" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C61" s="8" t="s">
         <v>64</v>
@@ -1968,7 +1968,7 @@
     <row r="62" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="20"/>
       <c r="B62" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C62" s="8" t="s">
         <v>15</v>
@@ -1980,7 +1980,7 @@
     <row r="63" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="20"/>
       <c r="B63" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C63" s="8" t="s">
         <v>6</v>
@@ -1992,7 +1992,7 @@
     <row r="64" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="20"/>
       <c r="B64" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C64" s="8" t="s">
         <v>64</v>
@@ -2004,7 +2004,7 @@
     <row r="65" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="20"/>
       <c r="B65" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C65" s="8" t="s">
         <v>15</v>
@@ -2016,7 +2016,7 @@
     <row r="66" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="20"/>
       <c r="B66" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C66" s="8" t="s">
         <v>64</v>
@@ -2028,7 +2028,7 @@
     <row r="67" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="20"/>
       <c r="B67" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C67" s="8" t="s">
         <v>64</v>
@@ -2040,7 +2040,7 @@
     <row r="68" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="20"/>
       <c r="B68" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C68" s="8" t="s">
         <v>6</v>
@@ -2052,7 +2052,7 @@
     <row r="69" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="20"/>
       <c r="B69" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C69" s="8" t="s">
         <v>15</v>
@@ -2064,7 +2064,7 @@
     <row r="70" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="20"/>
       <c r="B70" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C70" s="8" t="s">
         <v>15</v>
@@ -2076,7 +2076,7 @@
     <row r="71" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="20"/>
       <c r="B71" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C71" s="8" t="s">
         <v>6</v>
@@ -2088,7 +2088,7 @@
     <row r="72" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="20"/>
       <c r="B72" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C72" s="8" t="s">
         <v>15</v>
@@ -2100,7 +2100,7 @@
     <row r="73" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="20"/>
       <c r="B73" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C73" s="8" t="s">
         <v>15</v>
@@ -2112,7 +2112,7 @@
     <row r="74" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="20"/>
       <c r="B74" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C74" s="8" t="s">
         <v>15</v>
@@ -2124,7 +2124,7 @@
     <row r="75" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="20"/>
       <c r="B75" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C75" s="8" t="s">
         <v>15</v>
@@ -2136,7 +2136,7 @@
     <row r="76" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="20"/>
       <c r="B76" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C76" s="8" t="s">
         <v>64</v>
@@ -2148,7 +2148,7 @@
     <row r="77" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="20"/>
       <c r="B77" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C77" s="8" t="s">
         <v>15</v>
@@ -2160,7 +2160,7 @@
     <row r="78" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="20"/>
       <c r="B78" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C78" s="8" t="s">
         <v>15</v>
@@ -2172,7 +2172,7 @@
     <row r="79" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="20"/>
       <c r="B79" s="8" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C79" s="8" t="s">
         <v>64</v>
@@ -2184,7 +2184,7 @@
     <row r="80" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="20"/>
       <c r="B80" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C80" s="8" t="s">
         <v>64</v>
@@ -2196,7 +2196,7 @@
     <row r="81" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="20"/>
       <c r="B81" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C81" s="8" t="s">
         <v>64</v>
@@ -2208,7 +2208,7 @@
     <row r="82" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="20"/>
       <c r="B82" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C82" s="8" t="s">
         <v>64</v>
@@ -2220,7 +2220,7 @@
     <row r="83" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="20"/>
       <c r="B83" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C83" s="8" t="s">
         <v>64</v>
@@ -2232,7 +2232,7 @@
     <row r="84" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="20"/>
       <c r="B84" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C84" s="8" t="s">
         <v>64</v>
@@ -2244,7 +2244,7 @@
     <row r="85" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="21"/>
       <c r="B85" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C85" s="11" t="s">
         <v>64</v>
@@ -2277,10 +2277,10 @@
     </row>
     <row r="86" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="B86" s="6" t="s">
         <v>109</v>
-      </c>
-      <c r="B86" s="6" t="s">
-        <v>110</v>
       </c>
       <c r="C86" s="10" t="s">
         <v>64</v>
@@ -2292,7 +2292,7 @@
     <row r="87" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="20"/>
       <c r="B87" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C87" s="8" t="s">
         <v>6</v>
@@ -2304,7 +2304,7 @@
     <row r="88" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="20"/>
       <c r="B88" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C88" s="8" t="s">
         <v>6</v>
@@ -2316,7 +2316,7 @@
     <row r="89" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="21"/>
       <c r="B89" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C89" s="9" t="s">
         <v>6</v>
@@ -2349,10 +2349,10 @@
     </row>
     <row r="90" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="B90" s="5" t="s">
         <v>114</v>
-      </c>
-      <c r="B90" s="5" t="s">
-        <v>115</v>
       </c>
       <c r="C90" s="8" t="s">
         <v>6</v>
@@ -2364,7 +2364,7 @@
     <row r="91" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="20"/>
       <c r="B91" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C91" s="8" t="s">
         <v>6</v>
@@ -2376,7 +2376,7 @@
     <row r="92" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="20"/>
       <c r="B92" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C92" s="8" t="s">
         <v>6</v>
@@ -2388,7 +2388,7 @@
     <row r="93" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="20"/>
       <c r="B93" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C93" s="8" t="s">
         <v>6</v>
@@ -2400,7 +2400,7 @@
     <row r="94" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="20"/>
       <c r="B94" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C94" s="8" t="s">
         <v>6</v>
@@ -2412,7 +2412,7 @@
     <row r="95" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="20"/>
       <c r="B95" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C95" s="8" t="s">
         <v>6</v>
@@ -2424,7 +2424,7 @@
     <row r="96" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="20"/>
       <c r="B96" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C96" s="8" t="s">
         <v>6</v>
@@ -2436,7 +2436,7 @@
     <row r="97" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="20"/>
       <c r="B97" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C97" s="8" t="s">
         <v>6</v>
@@ -2448,7 +2448,7 @@
     <row r="98" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="20"/>
       <c r="B98" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C98" s="8" t="s">
         <v>6</v>
@@ -2460,7 +2460,7 @@
     <row r="99" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="20"/>
       <c r="B99" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C99" s="8" t="s">
         <v>6</v>
@@ -2472,7 +2472,7 @@
     <row r="100" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="20"/>
       <c r="B100" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C100" s="8" t="s">
         <v>6</v>
@@ -2484,7 +2484,7 @@
     <row r="101" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="20"/>
       <c r="B101" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C101" s="8" t="s">
         <v>6</v>
@@ -2496,7 +2496,7 @@
     <row r="102" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="20"/>
       <c r="B102" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C102" s="8" t="s">
         <v>6</v>
@@ -2508,7 +2508,7 @@
     <row r="103" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="20"/>
       <c r="B103" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C103" s="8" t="s">
         <v>6</v>
@@ -2520,7 +2520,7 @@
     <row r="104" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="20"/>
       <c r="B104" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C104" s="8" t="s">
         <v>6</v>
@@ -2532,7 +2532,7 @@
     <row r="105" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="20"/>
       <c r="B105" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C105" s="8" t="s">
         <v>6</v>
@@ -2544,7 +2544,7 @@
     <row r="106" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="20"/>
       <c r="B106" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C106" s="8" t="s">
         <v>6</v>
@@ -2556,7 +2556,7 @@
     <row r="107" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="20"/>
       <c r="B107" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C107" s="8" t="s">
         <v>6</v>
@@ -2568,7 +2568,7 @@
     <row r="108" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="20"/>
       <c r="B108" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C108" s="8" t="s">
         <v>6</v>
@@ -2580,7 +2580,7 @@
     <row r="109" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="20"/>
       <c r="B109" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C109" s="8" t="s">
         <v>6</v>
@@ -2592,7 +2592,7 @@
     <row r="110" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="20"/>
       <c r="B110" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C110" s="8" t="s">
         <v>6</v>
@@ -2604,7 +2604,7 @@
     <row r="111" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="20"/>
       <c r="B111" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C111" s="8" t="s">
         <v>6</v>
@@ -2616,7 +2616,7 @@
     <row r="112" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="20"/>
       <c r="B112" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C112" s="8" t="s">
         <v>6</v>
@@ -2628,7 +2628,7 @@
     <row r="113" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="20"/>
       <c r="B113" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C113" s="8" t="s">
         <v>6</v>
@@ -2640,7 +2640,7 @@
     <row r="114" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="20"/>
       <c r="B114" s="5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C114" s="8" t="s">
         <v>6</v>
@@ -2652,7 +2652,7 @@
     <row r="115" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="20"/>
       <c r="B115" s="5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C115" s="8" t="s">
         <v>6</v>
@@ -2664,7 +2664,7 @@
     <row r="116" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="20"/>
       <c r="B116" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C116" s="8" t="s">
         <v>6</v>
@@ -2676,7 +2676,7 @@
     <row r="117" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="20"/>
       <c r="B117" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C117" s="8" t="s">
         <v>6</v>
@@ -2688,7 +2688,7 @@
     <row r="118" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="20"/>
       <c r="B118" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C118" s="8" t="s">
         <v>6</v>
@@ -2700,7 +2700,7 @@
     <row r="119" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="20"/>
       <c r="B119" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C119" s="8" t="s">
         <v>6</v>
@@ -2712,7 +2712,7 @@
     <row r="120" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="20"/>
       <c r="B120" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C120" s="8" t="s">
         <v>6</v>
@@ -2724,7 +2724,7 @@
     <row r="121" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="20"/>
       <c r="B121" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C121" s="8" t="s">
         <v>6</v>
@@ -2736,7 +2736,7 @@
     <row r="122" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="20"/>
       <c r="B122" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C122" s="8" t="s">
         <v>6</v>
@@ -2748,7 +2748,7 @@
     <row r="123" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="21"/>
       <c r="B123" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C123" s="9" t="s">
         <v>6</v>
@@ -2781,10 +2781,10 @@
     </row>
     <row r="124" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="22" t="s">
+        <v>148</v>
+      </c>
+      <c r="B124" s="5" t="s">
         <v>149</v>
-      </c>
-      <c r="B124" s="5" t="s">
-        <v>150</v>
       </c>
       <c r="C124" s="8" t="s">
         <v>15</v>
@@ -2796,7 +2796,7 @@
     <row r="125" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="20"/>
       <c r="B125" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C125" s="8" t="s">
         <v>6</v>
@@ -2808,7 +2808,7 @@
     <row r="126" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="20"/>
       <c r="B126" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C126" s="8" t="s">
         <v>6</v>
@@ -2820,7 +2820,7 @@
     <row r="127" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="20"/>
       <c r="B127" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C127" s="8" t="s">
         <v>6</v>
@@ -2832,7 +2832,7 @@
     <row r="128" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="20"/>
       <c r="B128" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C128" s="8" t="s">
         <v>6</v>
@@ -2844,7 +2844,7 @@
     <row r="129" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="20"/>
       <c r="B129" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C129" s="8" t="s">
         <v>6</v>
@@ -2856,7 +2856,7 @@
     <row r="130" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="20"/>
       <c r="B130" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C130" s="8" t="s">
         <v>6</v>
@@ -2868,7 +2868,7 @@
     <row r="131" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="20"/>
       <c r="B131" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C131" s="8" t="s">
         <v>6</v>
@@ -2880,7 +2880,7 @@
     <row r="132" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="20"/>
       <c r="B132" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C132" s="8" t="s">
         <v>6</v>
@@ -2892,7 +2892,7 @@
     <row r="133" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="20"/>
       <c r="B133" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C133" s="8" t="s">
         <v>6</v>
@@ -2904,7 +2904,7 @@
     <row r="134" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="20"/>
       <c r="B134" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C134" s="8" t="s">
         <v>6</v>
@@ -2916,7 +2916,7 @@
     <row r="135" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="20"/>
       <c r="B135" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C135" s="8" t="s">
         <v>6</v>
@@ -2928,7 +2928,7 @@
     <row r="136" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="20"/>
       <c r="B136" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C136" s="8" t="s">
         <v>6</v>
@@ -2940,7 +2940,7 @@
     <row r="137" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="20"/>
       <c r="B137" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C137" s="8" t="s">
         <v>6</v>
@@ -2952,7 +2952,7 @@
     <row r="138" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" s="20"/>
       <c r="B138" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C138" s="8" t="s">
         <v>6</v>
@@ -2964,7 +2964,7 @@
     <row r="139" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="20"/>
       <c r="B139" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C139" s="8" t="s">
         <v>6</v>
@@ -2976,7 +2976,7 @@
     <row r="140" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="21"/>
       <c r="B140" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C140" s="9" t="s">
         <v>6</v>
@@ -3009,10 +3009,10 @@
     </row>
     <row r="141" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A141" s="16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B141" s="12" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C141" s="12" t="s">
         <v>64</v>
@@ -3021,25 +3021,25 @@
     <row r="142" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A142" s="17"/>
       <c r="B142" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="C142" s="12" t="s">
         <v>168</v>
-      </c>
-      <c r="C142" s="12" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="143" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A143" s="17"/>
       <c r="B143" s="12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C143" s="12" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="144" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A144" s="17"/>
       <c r="B144" s="12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C144" s="12" t="s">
         <v>64</v>
@@ -3048,7 +3048,7 @@
     <row r="145" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A145" s="17"/>
       <c r="B145" s="12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C145" s="12" t="s">
         <v>64</v>
@@ -3057,7 +3057,7 @@
     <row r="146" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A146" s="17"/>
       <c r="B146" s="12" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C146" s="12" t="s">
         <v>6</v>
@@ -3066,7 +3066,7 @@
     <row r="147" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A147" s="17"/>
       <c r="B147" s="12" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C147" s="12" t="s">
         <v>64</v>
@@ -3075,7 +3075,7 @@
     <row r="148" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A148" s="17"/>
       <c r="B148" s="12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C148" s="12" t="s">
         <v>64</v>
@@ -3084,7 +3084,7 @@
     <row r="149" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A149" s="17"/>
       <c r="B149" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C149" s="12" t="s">
         <v>64</v>
@@ -3093,7 +3093,7 @@
     <row r="150" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A150" s="17"/>
       <c r="B150" s="12" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C150" s="12" t="s">
         <v>64</v>
@@ -3102,7 +3102,7 @@
     <row r="151" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A151" s="17"/>
       <c r="B151" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C151" s="12" t="s">
         <v>64</v>
@@ -3111,7 +3111,7 @@
     <row r="152" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A152" s="17"/>
       <c r="B152" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C152" s="12" t="s">
         <v>64</v>
@@ -3120,7 +3120,7 @@
     <row r="153" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A153" s="17"/>
       <c r="B153" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C153" s="12" t="s">
         <v>64</v>
@@ -3129,7 +3129,7 @@
     <row r="154" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A154" s="17"/>
       <c r="B154" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C154" s="12" t="s">
         <v>64</v>
@@ -3138,7 +3138,7 @@
     <row r="155" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A155" s="17"/>
       <c r="B155" s="12" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C155" s="12" t="s">
         <v>64</v>
@@ -3147,7 +3147,7 @@
     <row r="156" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A156" s="17"/>
       <c r="B156" s="12" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C156" s="12" t="s">
         <v>64</v>
@@ -3156,7 +3156,7 @@
     <row r="157" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A157" s="17"/>
       <c r="B157" s="12" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C157" s="12" t="s">
         <v>64</v>
@@ -3165,7 +3165,7 @@
     <row r="158" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A158" s="17"/>
       <c r="B158" s="12" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C158" s="12" t="s">
         <v>64</v>
@@ -3174,7 +3174,7 @@
     <row r="159" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A159" s="17"/>
       <c r="B159" s="12" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C159" s="12" t="s">
         <v>64</v>
@@ -3183,7 +3183,7 @@
     <row r="160" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A160" s="17"/>
       <c r="B160" s="12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C160" s="12" t="s">
         <v>64</v>
@@ -3192,7 +3192,7 @@
     <row r="161" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A161" s="17"/>
       <c r="B161" s="12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C161" s="12" t="s">
         <v>64</v>
@@ -3201,7 +3201,7 @@
     <row r="162" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A162" s="17"/>
       <c r="B162" s="12" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C162" s="12" t="s">
         <v>64</v>
@@ -3210,7 +3210,7 @@
     <row r="163" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A163" s="17"/>
       <c r="B163" s="12" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C163" s="12" t="s">
         <v>64</v>
@@ -3219,7 +3219,7 @@
     <row r="164" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A164" s="17"/>
       <c r="B164" s="12" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C164" s="12" t="s">
         <v>64</v>
@@ -3228,7 +3228,7 @@
     <row r="165" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A165" s="17"/>
       <c r="B165" s="12" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C165" s="12" t="s">
         <v>64</v>
@@ -3237,7 +3237,7 @@
     <row r="166" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A166" s="17"/>
       <c r="B166" s="12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C166" s="12" t="s">
         <v>64</v>
@@ -3246,7 +3246,7 @@
     <row r="167" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A167" s="17"/>
       <c r="B167" s="12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C167" s="12" t="s">
         <v>64</v>
@@ -3255,7 +3255,7 @@
     <row r="168" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A168" s="17"/>
       <c r="B168" s="12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C168" s="12" t="s">
         <v>64</v>
@@ -3264,7 +3264,7 @@
     <row r="169" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A169" s="17"/>
       <c r="B169" s="12" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C169" s="12" t="s">
         <v>64</v>
@@ -3273,7 +3273,7 @@
     <row r="170" spans="1:3" s="14" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A170" s="18"/>
       <c r="B170" s="13" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C170" s="13" t="s">
         <v>64</v>

</xml_diff>